<commit_message>
This commit is for saved results for responses.
</commit_message>
<xml_diff>
--- a/filterbank harmonic summation model/FH/amp_FH.xlsx
+++ b/filterbank harmonic summation model/FH/amp_FH.xlsx
@@ -553,115 +553,115 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3065762777957007</v>
+        <v>4.828951287547961e-05</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3045925432286531</v>
+        <v>4.797705042207081e-05</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2872694929693623</v>
+        <v>4.524845816257428e-05</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2920343495135259</v>
+        <v>4.59989813377318e-05</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2626771030144431</v>
+        <v>4.137485600422902e-05</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2487568195113371</v>
+        <v>3.918224112128131e-05</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2133489732021551</v>
+        <v>3.360507232487606e-05</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1843280637306775</v>
+        <v>2.90339241862881e-05</v>
       </c>
       <c r="J2" t="n">
-        <v>0.12058357559671</v>
+        <v>1.899338777356098e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1451727036231029</v>
+        <v>2.286647613827321e-05</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1722783915804133</v>
+        <v>2.713595346712749e-05</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1768946041787132</v>
+        <v>2.786306340304399e-05</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1555266137237173</v>
+        <v>2.449734359713239e-05</v>
       </c>
       <c r="O2" t="n">
-        <v>0.1557907183665537</v>
+        <v>2.453894330811596e-05</v>
       </c>
       <c r="P2" t="n">
-        <v>0.1589739265439092</v>
+        <v>2.504033752351634e-05</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.1412797938149613</v>
+        <v>2.225329523707966e-05</v>
       </c>
       <c r="R2" t="n">
-        <v>0.1186450794344811</v>
+        <v>1.868805092213179e-05</v>
       </c>
       <c r="S2" t="n">
-        <v>0.1015212372538824</v>
+        <v>1.532768859827824e-05</v>
       </c>
       <c r="T2" t="n">
-        <v>0.05661000321414267</v>
+        <v>8.916767790207086e-06</v>
       </c>
       <c r="U2" t="n">
-        <v>0.07953285104016843</v>
+        <v>1.252739664641356e-05</v>
       </c>
       <c r="V2" t="n">
-        <v>0.09887919708660893</v>
+        <v>1.557468273527929e-05</v>
       </c>
       <c r="W2" t="n">
-        <v>0.0974672724994914</v>
+        <v>1.535228734637626e-05</v>
       </c>
       <c r="X2" t="n">
-        <v>0.08378753963771017</v>
+        <v>1.319756213113206e-05</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.06780297270506652</v>
+        <v>1.067979736390099e-05</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.1511831966274377</v>
+        <v>2.381320228880147e-05</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.0975209845179537</v>
+        <v>1.536074764612858e-05</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.2129381972618818</v>
+        <v>3.354037009090224e-05</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.2753731492141557</v>
+        <v>4.337463854068888e-05</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.2996920563458131</v>
+        <v>4.720516380994775e-05</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.2576505687554001</v>
+        <v>4.058311538892007e-05</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.1841593960478112</v>
+        <v>2.900735696359882e-05</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.1708797657785937</v>
+        <v>2.691565279953979e-05</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.1541112504694317</v>
+        <v>2.427440657609891e-05</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.1157096221109429</v>
+        <v>1.822568049595392e-05</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.1423087399061347</v>
+        <v>2.241536682942576e-05</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.1418462454281571</v>
+        <v>2.234251829329728e-05</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.1433783854469263</v>
+        <v>2.25838490828005e-05</v>
       </c>
     </row>
     <row r="3">
@@ -671,115 +671,115 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5349661612890237</v>
+        <v>8.426371250657307e-05</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5754937605741108</v>
+        <v>9.064730500616514e-05</v>
       </c>
       <c r="D3" t="n">
-        <v>0.594701849177997</v>
+        <v>9.367281385707768e-05</v>
       </c>
       <c r="E3" t="n">
-        <v>0.526874257549856</v>
+        <v>8.298913871172754e-05</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4164751882801103</v>
+        <v>6.559993523103635e-05</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3465429161353721</v>
+        <v>5.458474716617481e-05</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3013948824485145</v>
+        <v>4.747337974499115e-05</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2623931903235527</v>
+        <v>4.133013628344423e-05</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1890110936901693</v>
+        <v>2.977155867370214e-05</v>
       </c>
       <c r="K3" t="n">
-        <v>0.183757790560121</v>
+        <v>2.894409918805233e-05</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1551520540556622</v>
+        <v>2.443834586892187e-05</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1676945219332947</v>
+        <v>2.641393794154412e-05</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1419292098244404</v>
+        <v>2.235558620028387e-05</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1148276925900824</v>
+        <v>1.808676581129839e-05</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1669568181592542</v>
+        <v>2.629774057575004e-05</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1801852103520217</v>
+        <v>2.838137411617753e-05</v>
       </c>
       <c r="R3" t="n">
-        <v>0.07956697048565625</v>
+        <v>1.253277087632475e-05</v>
       </c>
       <c r="S3" t="n">
-        <v>0.1500906693438089</v>
+        <v>2.364111588110895e-05</v>
       </c>
       <c r="T3" t="n">
-        <v>0.1128555621086533</v>
+        <v>1.777613114328093e-05</v>
       </c>
       <c r="U3" t="n">
-        <v>0.08436305176256165</v>
+        <v>1.328128344864248e-05</v>
       </c>
       <c r="V3" t="n">
-        <v>0.09720219971697716</v>
+        <v>1.462551069125542e-05</v>
       </c>
       <c r="W3" t="n">
-        <v>0.09799669887074165</v>
+        <v>1.548953674800995e-05</v>
       </c>
       <c r="X3" t="n">
-        <v>0.09239267038236489</v>
+        <v>1.501292454032276e-05</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.2755134606242798</v>
+        <v>4.339673930365229e-05</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.224311758899279</v>
+        <v>3.533184513612784e-05</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.1908346918539003</v>
+        <v>3.005879768527978e-05</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.1391215101193961</v>
+        <v>2.191333916136728e-05</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.2912504438592554</v>
+        <v>4.587550661079848e-05</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.4185232483920829</v>
+        <v>6.592252974440821e-05</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.4458696626789772</v>
+        <v>7.022992441401527e-05</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.4287508373348922</v>
+        <v>6.753350007613106e-05</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.3234813605599388</v>
+        <v>5.095227014317896e-05</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.1841340583384947</v>
+        <v>2.900336596452652e-05</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.3209228818292866</v>
+        <v>5.054927845545353e-05</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.7211999887497434</v>
+        <v>0.0001135978177859359</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.6828534939289246</v>
+        <v>0.0001075577759122022</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.7075865051834919</v>
+        <v>0.0001114535276449006</v>
       </c>
     </row>
     <row r="4">
@@ -789,115 +789,115 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.154433681027869</v>
+        <v>2.432519333205752e-05</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1614456902441036</v>
+        <v>2.542967053350616e-05</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1537256017229641</v>
+        <v>2.421366218243003e-05</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2199561698998607</v>
+        <v>3.464578660420234e-05</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2547857709865627</v>
+        <v>4.013187470670359e-05</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2460316194072897</v>
+        <v>3.875298877840973e-05</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1992568774608073</v>
+        <v>3.138539491331265e-05</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1441872063233014</v>
+        <v>2.271124826190364e-05</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1428064195259311</v>
+        <v>2.249375745566997e-05</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1461986494744872</v>
+        <v>2.30280751561626e-05</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1550544186824961</v>
+        <v>2.442296710366479e-05</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1546358223788406</v>
+        <v>2.435703306682301e-05</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1151080919119819</v>
+        <v>1.813093213350212e-05</v>
       </c>
       <c r="O4" t="n">
-        <v>0.06647425587552815</v>
+        <v>1.047050821436471e-05</v>
       </c>
       <c r="P4" t="n">
-        <v>0.118296735904837</v>
+        <v>1.863318255631827e-05</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.1242982094622853</v>
+        <v>1.957848803366305e-05</v>
       </c>
       <c r="R4" t="n">
-        <v>0.1158452746341026</v>
+        <v>1.824704742724688e-05</v>
       </c>
       <c r="S4" t="n">
-        <v>0.09609972288095826</v>
+        <v>1.513688155768696e-05</v>
       </c>
       <c r="T4" t="n">
-        <v>0.08915382853216597</v>
+        <v>1.404281825637947e-05</v>
       </c>
       <c r="U4" t="n">
-        <v>0.08212570995843556</v>
+        <v>1.293580363412381e-05</v>
       </c>
       <c r="V4" t="n">
-        <v>0.08401100557966169</v>
+        <v>1.323276074975541e-05</v>
       </c>
       <c r="W4" t="n">
-        <v>0.09341953963875317</v>
+        <v>1.471471992106694e-05</v>
       </c>
       <c r="X4" t="n">
-        <v>0.08031081767924905</v>
+        <v>1.264993590582623e-05</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.06978831390548644</v>
+        <v>1.099251288171344e-05</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.04736421582939839</v>
+        <v>7.460443210335052e-06</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.1729489934150398</v>
+        <v>2.724158145687396e-05</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.2203642606858728</v>
+        <v>3.471006589354326e-05</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.2044435717579313</v>
+        <v>3.220236269321719e-05</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.1569825248592307</v>
+        <v>2.472666740531946e-05</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.6345396716352008</v>
+        <v>9.994775807099428e-05</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.6233524573272283</v>
+        <v>9.818563500899535e-05</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.4006325846016925</v>
+        <v>6.310453141241513e-05</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.3039423972320208</v>
+        <v>4.787464447696296e-05</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.2990884805931348</v>
+        <v>4.711009324777037e-05</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.2523549248350368</v>
+        <v>3.974898671100994e-05</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.3015764005539456</v>
+        <v>4.750197106638227e-05</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.463135907841111</v>
+        <v>7.294956917603979e-05</v>
       </c>
     </row>
     <row r="5">
@@ -907,115 +907,115 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2517150066401452</v>
+        <v>3.964819176975207e-05</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2110731781988145</v>
+        <v>3.324660678114277e-05</v>
       </c>
       <c r="D5" t="n">
-        <v>0.141657042928563</v>
+        <v>2.2312716585853e-05</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1245295096702184</v>
+        <v>1.961492064498378e-05</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1546070896590926</v>
+        <v>2.435250731209014e-05</v>
       </c>
       <c r="G5" t="n">
-        <v>0.166794542471674</v>
+        <v>2.627218017048605e-05</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1400091461325384</v>
+        <v>2.205315268834192e-05</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1047123156868242</v>
+        <v>1.649347024804635e-05</v>
       </c>
       <c r="J5" t="n">
-        <v>0.07026451013680927</v>
+        <v>1.106751961155261e-05</v>
       </c>
       <c r="K5" t="n">
-        <v>0.06518647235235024</v>
+        <v>1.026766656115379e-05</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1189043905683048</v>
+        <v>1.872889559682602e-05</v>
       </c>
       <c r="M5" t="n">
-        <v>0.06495093913019945</v>
+        <v>1.023056719832823e-05</v>
       </c>
       <c r="N5" t="n">
-        <v>0.07937890470858169</v>
+        <v>1.250314821657828e-05</v>
       </c>
       <c r="O5" t="n">
-        <v>0.07392730230125648</v>
+        <v>1.164445416975462e-05</v>
       </c>
       <c r="P5" t="n">
-        <v>0.06007981298949414</v>
+        <v>9.463305262144027e-06</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.04679986176914264</v>
+        <v>7.371550544356471e-06</v>
       </c>
       <c r="R5" t="n">
-        <v>0.05206616577214405</v>
+        <v>8.201057826484134e-06</v>
       </c>
       <c r="S5" t="n">
-        <v>0.05369677996079751</v>
+        <v>8.457899501985179e-06</v>
       </c>
       <c r="T5" t="n">
-        <v>0.09451604156098531</v>
+        <v>1.488743238294535e-05</v>
       </c>
       <c r="U5" t="n">
-        <v>0.1138123729313864</v>
+        <v>1.792684054870518e-05</v>
       </c>
       <c r="V5" t="n">
-        <v>0.1262930825589506</v>
+        <v>1.989270494169975e-05</v>
       </c>
       <c r="W5" t="n">
-        <v>0.1154867247620869</v>
+        <v>1.819057143769645e-05</v>
       </c>
       <c r="X5" t="n">
-        <v>0.09509357551005222</v>
+        <v>1.497840104258861e-05</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.06554539515222747</v>
+        <v>1.032420129140296e-05</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.1705779709004253</v>
+        <v>2.686811641557736e-05</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.2340786865856162</v>
+        <v>3.687025568652783e-05</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.2608248533542261</v>
+        <v>4.108310403157556e-05</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.2997038441696865</v>
+        <v>4.720702053636117e-05</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.3139039059238673</v>
+        <v>4.944370391526261e-05</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.2589529923743409</v>
+        <v>4.078826303624744e-05</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.2245989183359505</v>
+        <v>3.537707625907763e-05</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.2907714622666399</v>
+        <v>4.580006115249352e-05</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.2762199484858871</v>
+        <v>4.35080197814986e-05</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.2240685480896057</v>
+        <v>3.529353645937824e-05</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.1731423828539083</v>
+        <v>2.727204265845605e-05</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.1608953446523577</v>
+        <v>2.534298437262751e-05</v>
       </c>
       <c r="AL5" t="n">
-        <v>0.1639733168463257</v>
+        <v>2.582780263371304e-05</v>
       </c>
     </row>
     <row r="6">
@@ -1025,115 +1025,115 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.07503982489212366</v>
+        <v>1.181969008285988e-05</v>
       </c>
       <c r="C6" t="n">
-        <v>0.08412799626437452</v>
+        <v>1.325118821327729e-05</v>
       </c>
       <c r="D6" t="n">
-        <v>0.09990081893410716</v>
+        <v>1.573560066967835e-05</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1269294308084501</v>
+        <v>1.999293757290148e-05</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1486559534182079</v>
+        <v>2.341513057767941e-05</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1685388988605994</v>
+        <v>2.654693763348379e-05</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1576252324605455</v>
+        <v>2.482790171220063e-05</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1360298566120665</v>
+        <v>2.142636592611846e-05</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1014767906744586</v>
+        <v>1.598383549134908e-05</v>
       </c>
       <c r="K6" t="n">
-        <v>0.09151788908444562</v>
+        <v>1.441518670347046e-05</v>
       </c>
       <c r="L6" t="n">
-        <v>0.07448701317883125</v>
+        <v>1.173261547767944e-05</v>
       </c>
       <c r="M6" t="n">
-        <v>0.02928516022888662</v>
+        <v>4.612770864403571e-06</v>
       </c>
       <c r="N6" t="n">
-        <v>0.05065690835999709</v>
+        <v>7.979082550255862e-06</v>
       </c>
       <c r="O6" t="n">
-        <v>0.08132754742549954</v>
+        <v>1.281008327445325e-05</v>
       </c>
       <c r="P6" t="n">
-        <v>0.08904922214999778</v>
+        <v>1.402634147195607e-05</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.08245155999503029</v>
+        <v>1.298712899970902e-05</v>
       </c>
       <c r="R6" t="n">
-        <v>0.06607397605981659</v>
+        <v>1.04074592483665e-05</v>
       </c>
       <c r="S6" t="n">
-        <v>0.04969872563209108</v>
+        <v>7.828157052989849e-06</v>
       </c>
       <c r="T6" t="n">
-        <v>0.03398915302280364</v>
+        <v>5.242510432054076e-06</v>
       </c>
       <c r="U6" t="n">
-        <v>0.04077054874089515</v>
+        <v>6.273139515409326e-06</v>
       </c>
       <c r="V6" t="n">
-        <v>0.03982663139272771</v>
+        <v>6.29906905779472e-06</v>
       </c>
       <c r="W6" t="n">
-        <v>0.03696553678900214</v>
+        <v>5.822524095980679e-06</v>
       </c>
       <c r="X6" t="n">
-        <v>0.04087459096306033</v>
+        <v>6.438247932235624e-06</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.03706945664228774</v>
+        <v>5.838892743709507e-06</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.05764798972865442</v>
+        <v>9.080263359784362e-06</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.1424272385653148</v>
+        <v>2.243403181736726e-05</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.1853593619949266</v>
+        <v>2.919636627465837e-05</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.2239582818351713</v>
+        <v>3.527616817585832e-05</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.2223994434533638</v>
+        <v>3.503063206768216e-05</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.2065625785187615</v>
+        <v>3.253613217139099e-05</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.1708892431666574</v>
+        <v>2.691714560405884e-05</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.121024923346397</v>
+        <v>1.906290544138026e-05</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.08829311465829662</v>
+        <v>1.390724529557127e-05</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.1884106754532571</v>
+        <v>2.96769854588712e-05</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.1838349482315642</v>
+        <v>2.895625246486614e-05</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.1857272829228108</v>
+        <v>2.925431832010678e-05</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.1542895342489687</v>
+        <v>2.430248845160911e-05</v>
       </c>
     </row>
     <row r="7">
@@ -1143,115 +1143,115 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5389736405790991</v>
+        <v>8.48949395022419e-05</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5908056329903653</v>
+        <v>9.305911216068069e-05</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6068757803434944</v>
+        <v>9.559035689070161e-05</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6304953273596371</v>
+        <v>9.931072438928895e-05</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6637519581620701</v>
+        <v>0.0001045490504361573</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6569630507588895</v>
+        <v>0.0001034797144985777</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6538600588630874</v>
+        <v>0.0001029909553284873</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5707705584953802</v>
+        <v>8.990334291870596e-05</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4231252076692522</v>
+        <v>6.66473946079427e-05</v>
       </c>
       <c r="K7" t="n">
-        <v>0.2760146380258547</v>
+        <v>4.347568087330098e-05</v>
       </c>
       <c r="L7" t="n">
-        <v>0.184799743763984</v>
+        <v>2.910821955971109e-05</v>
       </c>
       <c r="M7" t="n">
-        <v>0.07020067480921995</v>
+        <v>1.105746476681479e-05</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2075158182177503</v>
+        <v>3.268627908115421e-05</v>
       </c>
       <c r="O7" t="n">
-        <v>0.1687690888432349</v>
+        <v>2.65831953707432e-05</v>
       </c>
       <c r="P7" t="n">
-        <v>0.1073073083654214</v>
+        <v>1.690221332910234e-05</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.1271745588968353</v>
+        <v>2.003154824449463e-05</v>
       </c>
       <c r="R7" t="n">
-        <v>0.1939920954256289</v>
+        <v>3.055612735972928e-05</v>
       </c>
       <c r="S7" t="n">
-        <v>0.20495401562389</v>
+        <v>3.228276384432598e-05</v>
       </c>
       <c r="T7" t="n">
-        <v>0.1577145622642385</v>
+        <v>2.425235216893432e-05</v>
       </c>
       <c r="U7" t="n">
-        <v>0.1217294768731293</v>
+        <v>1.917388123782878e-05</v>
       </c>
       <c r="V7" t="n">
-        <v>0.1507883518359633</v>
+        <v>2.375100940558555e-05</v>
       </c>
       <c r="W7" t="n">
-        <v>0.1879113048202848</v>
+        <v>2.959832847737238e-05</v>
       </c>
       <c r="X7" t="n">
-        <v>0.199960268817502</v>
+        <v>3.149618765376809e-05</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.1760319040183015</v>
+        <v>2.772717757781508e-05</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.2473604864944607</v>
+        <v>3.896230159536064e-05</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.5068672729353662</v>
+        <v>7.983779396944209e-05</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.7137117895868523</v>
+        <v>0.0001124183348445599</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.8204596705191771</v>
+        <v>0.0001292324315117089</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.7891297654512719</v>
+        <v>0.0001242975883299663</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.7442319453967344</v>
+        <v>0.0001172256326157367</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.6900856603143081</v>
+        <v>0.0001086969305600948</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.4033070805463723</v>
+        <v>6.352579723012492e-05</v>
       </c>
       <c r="AH7" t="n">
-        <v>0.4648080156180169</v>
+        <v>7.321294659911588e-05</v>
       </c>
       <c r="AI7" t="n">
-        <v>0.3937695177061977</v>
+        <v>6.202351444789929e-05</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.6616500760136027</v>
+        <v>0.0001042179782938476</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.7175084958495486</v>
+        <v>0.0001130163625108722</v>
       </c>
       <c r="AL7" t="n">
-        <v>0.2232898919215767</v>
+        <v>3.517088859072396e-05</v>
       </c>
     </row>
     <row r="8">
@@ -1261,115 +1261,115 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.2446855726399447</v>
+        <v>3.854096995174102e-05</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2723188119248849</v>
+        <v>4.28935430661245e-05</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2708449043363849</v>
+        <v>4.266138459651333e-05</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2344126610684704</v>
+        <v>3.692286075175279e-05</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1687459354786656</v>
+        <v>2.657954843268094e-05</v>
       </c>
       <c r="G8" t="n">
-        <v>0.109791842002685</v>
+        <v>1.72935577603442e-05</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1631466074109157</v>
+        <v>2.569758578780264e-05</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1867626965244263</v>
+        <v>2.941740862443875e-05</v>
       </c>
       <c r="J8" t="n">
-        <v>0.195337112845605</v>
+        <v>3.076798405159948e-05</v>
       </c>
       <c r="K8" t="n">
-        <v>0.1692121488169173</v>
+        <v>2.665298273478055e-05</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1085110441051156</v>
+        <v>1.709181642859386e-05</v>
       </c>
       <c r="M8" t="n">
-        <v>0.1247091331029772</v>
+        <v>1.964321353225905e-05</v>
       </c>
       <c r="N8" t="n">
-        <v>0.1175653009624596</v>
+        <v>1.851797260817269e-05</v>
       </c>
       <c r="O8" t="n">
-        <v>0.1183943605738281</v>
+        <v>1.864855963553688e-05</v>
       </c>
       <c r="P8" t="n">
-        <v>0.1156253451962707</v>
+        <v>1.821240585127029e-05</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.1145916017859791</v>
+        <v>1.804957862249664e-05</v>
       </c>
       <c r="R8" t="n">
-        <v>0.0970068622507687</v>
+        <v>1.527976710184346e-05</v>
       </c>
       <c r="S8" t="n">
-        <v>0.07695407516637438</v>
+        <v>1.212120791042944e-05</v>
       </c>
       <c r="T8" t="n">
-        <v>0.06140643983053316</v>
+        <v>9.672265212933176e-06</v>
       </c>
       <c r="U8" t="n">
-        <v>0.06420019575625494</v>
+        <v>1.011231593608793e-05</v>
       </c>
       <c r="V8" t="n">
-        <v>0.06487792267538151</v>
+        <v>1.021906621377585e-05</v>
       </c>
       <c r="W8" t="n">
-        <v>0.08319644580859821</v>
+        <v>1.310445762455788e-05</v>
       </c>
       <c r="X8" t="n">
-        <v>0.0885110786961105</v>
+        <v>1.394157729701014e-05</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.112786659967049</v>
+        <v>1.776527821337365e-05</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.1881270957461939</v>
+        <v>2.963231818711124e-05</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.2633116346709938</v>
+        <v>4.147480249982618e-05</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.2986873158905461</v>
+        <v>4.704690490126774e-05</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.2785777111985824</v>
+        <v>4.387939624183875e-05</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.227606233174256</v>
+        <v>3.585076512257722e-05</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.1779481935745033</v>
+        <v>2.802901661723031e-05</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.242091162706051</v>
+        <v>3.813231866010221e-05</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.2041503736966954</v>
+        <v>3.215618041305215e-05</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.13104756080283</v>
+        <v>2.064159340764623e-05</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.2066893628327862</v>
+        <v>3.255610225129581e-05</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.1843775240703065</v>
+        <v>2.904171479463039e-05</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.3044333871506442</v>
+        <v>4.795198139346403e-05</v>
       </c>
       <c r="AL8" t="n">
-        <v>0.3545308071878178</v>
+        <v>5.584293769089001e-05</v>
       </c>
     </row>
     <row r="9">
@@ -1379,115 +1379,115 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.5338971978671682</v>
+        <v>8.409533769527242e-05</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5373324202239792</v>
+        <v>8.463642722581952e-05</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3980012319578162</v>
+        <v>6.269006119218147e-05</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2670004765574544</v>
+        <v>4.205584020780747e-05</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1944050070395919</v>
+        <v>3.06211659884264e-05</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1999064027707897</v>
+        <v>3.148770309268279e-05</v>
       </c>
       <c r="H9" t="n">
-        <v>0.2054265690537929</v>
+        <v>3.235719678839366e-05</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1729823466128443</v>
+        <v>2.724683499340457e-05</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3215471339045758</v>
+        <v>5.064760579129298e-05</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1003635333012345</v>
+        <v>1.580848384103694e-05</v>
       </c>
       <c r="L9" t="n">
-        <v>0.5480594904909116</v>
+        <v>8.632607197425112e-05</v>
       </c>
       <c r="M9" t="n">
-        <v>0.2444058530705159</v>
+        <v>3.849691069886413e-05</v>
       </c>
       <c r="N9" t="n">
-        <v>0.2374500639008154</v>
+        <v>3.74012888422598e-05</v>
       </c>
       <c r="O9" t="n">
-        <v>0.2354012509095942</v>
+        <v>3.707857574119931e-05</v>
       </c>
       <c r="P9" t="n">
-        <v>0.2791527760360297</v>
+        <v>4.396997598620713e-05</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.2698877813228345</v>
+        <v>4.251062601721758e-05</v>
       </c>
       <c r="R9" t="n">
-        <v>0.2205015935821176</v>
+        <v>3.473169750414642e-05</v>
       </c>
       <c r="S9" t="n">
-        <v>0.1647140190931299</v>
+        <v>2.594447229563575e-05</v>
       </c>
       <c r="T9" t="n">
-        <v>0.08058945987905669</v>
+        <v>1.269382545981263e-05</v>
       </c>
       <c r="U9" t="n">
-        <v>0.05189180888907653</v>
+        <v>8.173594485189904e-06</v>
       </c>
       <c r="V9" t="n">
-        <v>0.1178210045503445</v>
+        <v>1.855824905026487e-05</v>
       </c>
       <c r="W9" t="n">
-        <v>0.1582646663137555</v>
+        <v>2.492862036372064e-05</v>
       </c>
       <c r="X9" t="n">
-        <v>0.1607292342244053</v>
+        <v>2.531681994885986e-05</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.1564461075945382</v>
+        <v>2.464217512628129e-05</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.2301732907996701</v>
+        <v>3.625510809113898e-05</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.3659750074944862</v>
+        <v>5.764553919036645e-05</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.4798329648801213</v>
+        <v>7.557955984806827e-05</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.5184936928858933</v>
+        <v>8.16690972911911e-05</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.5427307057946602</v>
+        <v>8.54867232188599e-05</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.5037835889788974</v>
+        <v>7.935207603591352e-05</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.3920154022185078</v>
+        <v>6.174721980750206e-05</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.2737202123087232</v>
+        <v>4.311428076431052e-05</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.2086690818016445</v>
+        <v>3.286793219888301e-05</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.1704914183148154</v>
+        <v>2.685448332489185e-05</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.1731205334254492</v>
+        <v>2.726860110627699e-05</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.1380819253479966</v>
+        <v>2.174959184678509e-05</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.4947764952850772</v>
+        <v>7.793334863134822e-05</v>
       </c>
     </row>
     <row r="10">
@@ -1497,115 +1497,115 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2661772918681765</v>
+        <v>4.192617855251699e-05</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3536129689597344</v>
+        <v>5.569836694571914e-05</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3894384415589243</v>
+        <v>6.134131698995438e-05</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4033297794583828</v>
+        <v>6.352937258635169e-05</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3736355296314695</v>
+        <v>5.885216510750039e-05</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3301443978278232</v>
+        <v>5.200177999518298e-05</v>
       </c>
       <c r="H10" t="n">
-        <v>0.2487555051579273</v>
+        <v>3.918203409454604e-05</v>
       </c>
       <c r="I10" t="n">
-        <v>0.08417810449630883</v>
+        <v>1.325908087258073e-05</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1133482078424863</v>
+        <v>1.785372887092649e-05</v>
       </c>
       <c r="K10" t="n">
-        <v>0.1297846827263183</v>
+        <v>2.044267466685405e-05</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1283937529322821</v>
+        <v>2.022358621460676e-05</v>
       </c>
       <c r="M10" t="n">
-        <v>0.09583259944924472</v>
+        <v>1.509480635053845e-05</v>
       </c>
       <c r="N10" t="n">
-        <v>0.1201756556888366</v>
+        <v>1.892913539961657e-05</v>
       </c>
       <c r="O10" t="n">
-        <v>0.1367135125581509</v>
+        <v>2.153405009805834e-05</v>
       </c>
       <c r="P10" t="n">
-        <v>0.1464350418119206</v>
+        <v>2.306530984015129e-05</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.1209933674843949</v>
+        <v>1.905793500721816e-05</v>
       </c>
       <c r="R10" t="n">
-        <v>0.1134038164581924</v>
+        <v>1.694471118238111e-05</v>
       </c>
       <c r="S10" t="n">
-        <v>0.1430714993660879</v>
+        <v>2.253551077215721e-05</v>
       </c>
       <c r="T10" t="n">
-        <v>0.1398639203160543</v>
+        <v>2.203027784627853e-05</v>
       </c>
       <c r="U10" t="n">
-        <v>0.1166946360050091</v>
+        <v>1.838083223000862e-05</v>
       </c>
       <c r="V10" t="n">
-        <v>0.1007737914007924</v>
+        <v>1.587310450876543e-05</v>
       </c>
       <c r="W10" t="n">
-        <v>0.0850041406429668</v>
+        <v>1.406780409533093e-05</v>
       </c>
       <c r="X10" t="n">
-        <v>0.1016475385151322</v>
+        <v>1.601073036433127e-05</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.1283270327878681</v>
+        <v>2.021307697594061e-05</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.1584699804610915</v>
+        <v>2.496095985271366e-05</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.3813566245378491</v>
+        <v>6.006833197655894e-05</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.4515463099178473</v>
+        <v>7.112406577388149e-05</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.4700767786717482</v>
+        <v>7.404284121180522e-05</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.4593566877361403</v>
+        <v>7.235429579340754e-05</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.3718358083299192</v>
+        <v>5.856868699370647e-05</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.3626461715247974</v>
+        <v>5.712120681679066e-05</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.3327429712801405</v>
+        <v>5.241108709188919e-05</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.2885525314638393</v>
+        <v>4.545055241573784e-05</v>
       </c>
       <c r="AI10" t="n">
-        <v>0.2235399628620307</v>
+        <v>3.521027782196409e-05</v>
       </c>
       <c r="AJ10" t="n">
-        <v>0.2768195200993718</v>
+        <v>4.360245964278635e-05</v>
       </c>
       <c r="AK10" t="n">
-        <v>0.3300131170019472</v>
+        <v>5.198110165967371e-05</v>
       </c>
       <c r="AL10" t="n">
-        <v>0.4221721776912651</v>
+        <v>6.649728073180194e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1615,115 +1615,115 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.5240862003550626</v>
+        <v>8.254998560838383e-05</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5308218845261179</v>
+        <v>8.361093823603655e-05</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5096509535985171</v>
+        <v>8.027625771553148e-05</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4809201493297496</v>
+        <v>7.575080469406819e-05</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4468735385850473</v>
+        <v>7.038804714562423e-05</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3846710452640676</v>
+        <v>6.059039377300407e-05</v>
       </c>
       <c r="H11" t="n">
-        <v>0.3101290098407216</v>
+        <v>4.884911161894628e-05</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2390723856779049</v>
+        <v>3.765682436153157e-05</v>
       </c>
       <c r="J11" t="n">
-        <v>0.1881022789543725</v>
+        <v>2.962840923891473e-05</v>
       </c>
       <c r="K11" t="n">
-        <v>0.2658564820822733</v>
+        <v>4.187564708805296e-05</v>
       </c>
       <c r="L11" t="n">
-        <v>0.2813153174119533</v>
+        <v>4.431060269864314e-05</v>
       </c>
       <c r="M11" t="n">
-        <v>0.2643993696464364</v>
+        <v>4.164613406037422e-05</v>
       </c>
       <c r="N11" t="n">
-        <v>0.1934659100339431</v>
+        <v>3.047324672581528e-05</v>
       </c>
       <c r="O11" t="n">
-        <v>0.2037051658646466</v>
+        <v>3.208605473505592e-05</v>
       </c>
       <c r="P11" t="n">
-        <v>0.2004039313222202</v>
+        <v>3.156606992381193e-05</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.2280207736762087</v>
+        <v>3.591606032105239e-05</v>
       </c>
       <c r="R11" t="n">
-        <v>0.2105247656969517</v>
+        <v>3.316022510556048e-05</v>
       </c>
       <c r="S11" t="n">
-        <v>0.1457095752169478</v>
+        <v>2.295103997970889e-05</v>
       </c>
       <c r="T11" t="n">
-        <v>0.1103102414708714</v>
+        <v>1.737521201609295e-05</v>
       </c>
       <c r="U11" t="n">
-        <v>0.1463651185208192</v>
+        <v>2.30542960667106e-05</v>
       </c>
       <c r="V11" t="n">
-        <v>0.1431796030831894</v>
+        <v>2.255253842960152e-05</v>
       </c>
       <c r="W11" t="n">
-        <v>0.1446379028631836</v>
+        <v>2.278223847850506e-05</v>
       </c>
       <c r="X11" t="n">
-        <v>0.1269146575293518</v>
+        <v>1.999061060078101e-05</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.1017940414141299</v>
+        <v>1.603380636250801e-05</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.1853197577368778</v>
+        <v>2.919012811969503e-05</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.2305463433475079</v>
+        <v>3.631386842948469e-05</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.3286421743633541</v>
+        <v>5.176516142883168e-05</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.4119207815247172</v>
+        <v>6.488256047120159e-05</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.4324233821066801</v>
+        <v>6.811197078925393e-05</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.4182004052231822</v>
+        <v>6.587167799725581e-05</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.3120019674441298</v>
+        <v>4.914412534588989e-05</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.2271687037914046</v>
+        <v>3.578184889422934e-05</v>
       </c>
       <c r="AH11" t="n">
-        <v>0.161717601274319</v>
+        <v>2.547249984596628e-05</v>
       </c>
       <c r="AI11" t="n">
-        <v>0.1511776536451193</v>
+        <v>2.381232920130117e-05</v>
       </c>
       <c r="AJ11" t="n">
-        <v>0.1291724628899105</v>
+        <v>2.034624255578074e-05</v>
       </c>
       <c r="AK11" t="n">
-        <v>0.173193703288835</v>
+        <v>2.728012625455484e-05</v>
       </c>
       <c r="AL11" t="n">
-        <v>0.1688352978152408</v>
+        <v>2.659362409350394e-05</v>
       </c>
     </row>
     <row r="12">
@@ -1733,115 +1733,115 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3629213231031602</v>
+        <v>5.716454655521267e-05</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3575016358383747</v>
+        <v>5.631087953362943e-05</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3672070777902188</v>
+        <v>5.783960532893741e-05</v>
       </c>
       <c r="E12" t="n">
-        <v>0.383658089328254</v>
+        <v>6.04308408256708e-05</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3564588804541</v>
+        <v>5.614663280874597e-05</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3134554802203335</v>
+        <v>4.937307138315612e-05</v>
       </c>
       <c r="H12" t="n">
-        <v>0.289739761566413</v>
+        <v>4.563755567553537e-05</v>
       </c>
       <c r="I12" t="n">
-        <v>0.2067978030512959</v>
+        <v>3.257318291182701e-05</v>
       </c>
       <c r="J12" t="n">
-        <v>0.1452573748607747</v>
+        <v>2.287981289365146e-05</v>
       </c>
       <c r="K12" t="n">
-        <v>0.1559561238702817</v>
+        <v>2.456499669769776e-05</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1340482217414858</v>
+        <v>2.11142342005804e-05</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0838286188378658</v>
+        <v>1.320403260751429e-05</v>
       </c>
       <c r="N12" t="n">
-        <v>0.08175889615109558</v>
+        <v>1.287802597370009e-05</v>
       </c>
       <c r="O12" t="n">
-        <v>0.09439263847467859</v>
+        <v>1.486799488775515e-05</v>
       </c>
       <c r="P12" t="n">
-        <v>0.1336631209477972</v>
+        <v>2.105357611617513e-05</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.1401365459136215</v>
+        <v>2.2073219711835e-05</v>
       </c>
       <c r="R12" t="n">
-        <v>0.08911184759032545</v>
+        <v>1.403620574465446e-05</v>
       </c>
       <c r="S12" t="n">
-        <v>0.08921392165225121</v>
+        <v>1.405228365767192e-05</v>
       </c>
       <c r="T12" t="n">
-        <v>0.08570411571790572</v>
+        <v>1.349944630158022e-05</v>
       </c>
       <c r="U12" t="n">
-        <v>0.1544779976163833</v>
+        <v>2.433217373669626e-05</v>
       </c>
       <c r="V12" t="n">
-        <v>0.1908444970091788</v>
+        <v>3.006034211714344e-05</v>
       </c>
       <c r="W12" t="n">
-        <v>0.1866571764832311</v>
+        <v>2.940078792754544e-05</v>
       </c>
       <c r="X12" t="n">
-        <v>0.142543122203213</v>
+        <v>2.245228490747775e-05</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.1097586354162435</v>
+        <v>1.728832731689616e-05</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.2608183329883283</v>
+        <v>4.108207699420908e-05</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.2596711018573155</v>
+        <v>4.090137406157997e-05</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.3302658841360468</v>
+        <v>5.202091557438479e-05</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.4561666870900742</v>
+        <v>7.185183168112012e-05</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.4394851709796035</v>
+        <v>6.922428889538671e-05</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.3661179761209689</v>
+        <v>5.766805849740143e-05</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.2626866839992441</v>
+        <v>4.137636512650107e-05</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.1809526385331828</v>
+        <v>2.850225343959302e-05</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.2661104278820015</v>
+        <v>4.191564665701445e-05</v>
       </c>
       <c r="AI12" t="n">
-        <v>0.2323594705890906</v>
+        <v>3.659945814277501e-05</v>
       </c>
       <c r="AJ12" t="n">
-        <v>0.2404006035649666</v>
+        <v>3.786603492152621e-05</v>
       </c>
       <c r="AK12" t="n">
-        <v>0.262428205323039</v>
+        <v>4.133565157406191e-05</v>
       </c>
       <c r="AL12" t="n">
-        <v>0.1428716785696283</v>
+        <v>2.250403655310542e-05</v>
       </c>
     </row>
     <row r="13">
@@ -1851,115 +1851,115 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1900853245958451</v>
+        <v>2.994076317812058e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1984697770571517</v>
+        <v>3.126141697428259e-05</v>
       </c>
       <c r="D13" t="n">
-        <v>0.15625397074375</v>
+        <v>2.461191122263974e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1493615093909166</v>
+        <v>2.352626427162812e-05</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1615603251659656</v>
+        <v>2.544772693557041e-05</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1704698814618315</v>
+        <v>2.685109100717261e-05</v>
       </c>
       <c r="H13" t="n">
-        <v>0.141448614764721</v>
+        <v>2.227988660117895e-05</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1246388650766452</v>
+        <v>1.963214545880374e-05</v>
       </c>
       <c r="J13" t="n">
-        <v>0.07759667308733514</v>
+        <v>1.222242494131358e-05</v>
       </c>
       <c r="K13" t="n">
-        <v>0.1017296924339146</v>
+        <v>1.602367061120014e-05</v>
       </c>
       <c r="L13" t="n">
-        <v>0.1100754896686828</v>
+        <v>1.733823573646741e-05</v>
       </c>
       <c r="M13" t="n">
-        <v>0.1080656876994248</v>
+        <v>1.702166734843211e-05</v>
       </c>
       <c r="N13" t="n">
-        <v>0.1193936158556998</v>
+        <v>1.880595456232893e-05</v>
       </c>
       <c r="O13" t="n">
-        <v>0.1108198132439819</v>
+        <v>7.629772282144843e-06</v>
       </c>
       <c r="P13" t="n">
-        <v>0.058445902297301</v>
+        <v>9.205944347022529e-06</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.05932456225838489</v>
+        <v>9.344344036029788e-06</v>
       </c>
       <c r="R13" t="n">
-        <v>0.05519013296542089</v>
+        <v>8.693120862433856e-06</v>
       </c>
       <c r="S13" t="n">
-        <v>0.05397741918242259</v>
+        <v>8.50210361132941e-06</v>
       </c>
       <c r="T13" t="n">
-        <v>0.05381069103176738</v>
+        <v>8.475841888681921e-06</v>
       </c>
       <c r="U13" t="n">
-        <v>0.05849748244314231</v>
+        <v>9.214068850766366e-06</v>
       </c>
       <c r="V13" t="n">
-        <v>0.07489321445381017</v>
+        <v>1.179659714592581e-05</v>
       </c>
       <c r="W13" t="n">
-        <v>0.08339110039894654</v>
+        <v>1.313511810296959e-05</v>
       </c>
       <c r="X13" t="n">
-        <v>0.07670328501094517</v>
+        <v>1.208170539403542e-05</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.0652294622751023</v>
+        <v>1.02744379997112e-05</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.1341313731325016</v>
+        <v>2.112733156152412e-05</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.1489154590122466</v>
+        <v>2.345600588223556e-05</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.1680229610525263</v>
+        <v>2.646567111930654e-05</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.2274775823244998</v>
+        <v>3.583050104046879e-05</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.2624154690386411</v>
+        <v>4.133364545351715e-05</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.2781154360320002</v>
+        <v>4.3806582249937e-05</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.2337297635872114</v>
+        <v>3.681529604729819e-05</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.1901037203426005</v>
+        <v>2.994366073319623e-05</v>
       </c>
       <c r="AH13" t="n">
-        <v>0.2408823620309679</v>
+        <v>3.794191777134781e-05</v>
       </c>
       <c r="AI13" t="n">
-        <v>0.2447505026875414</v>
+        <v>3.855119722826735e-05</v>
       </c>
       <c r="AJ13" t="n">
-        <v>0.194708252590694</v>
+        <v>3.066893087111617e-05</v>
       </c>
       <c r="AK13" t="n">
-        <v>0.2178390607467227</v>
+        <v>3.431231602244591e-05</v>
       </c>
       <c r="AL13" t="n">
-        <v>0.1456830030410658</v>
+        <v>2.294685453705621e-05</v>
       </c>
     </row>
     <row r="14">
@@ -1969,115 +1969,115 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.1808639037812147</v>
+        <v>2.848827663102038e-05</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2366605763280001</v>
+        <v>3.727693489489436e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2251110626682173</v>
+        <v>3.545774525442497e-05</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2237120569608912</v>
+        <v>3.523738474707412e-05</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2093540466482695</v>
+        <v>3.297582253866461e-05</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1876306643553189</v>
+        <v>2.955412417218677e-05</v>
       </c>
       <c r="H14" t="n">
-        <v>0.1481227011553945</v>
+        <v>2.333113682514201e-05</v>
       </c>
       <c r="I14" t="n">
-        <v>0.09725044369865467</v>
+        <v>1.531813415864411e-05</v>
       </c>
       <c r="J14" t="n">
-        <v>0.1003670370072847</v>
+        <v>1.580903571758669e-05</v>
       </c>
       <c r="K14" t="n">
-        <v>0.1374485523035298</v>
+        <v>2.164982784675981e-05</v>
       </c>
       <c r="L14" t="n">
-        <v>0.1928228779129792</v>
+        <v>3.037196130312082e-05</v>
       </c>
       <c r="M14" t="n">
-        <v>0.2242317861682862</v>
+        <v>3.53192484530096e-05</v>
       </c>
       <c r="N14" t="n">
-        <v>0.2215787542653031</v>
+        <v>3.490136348435089e-05</v>
       </c>
       <c r="O14" t="n">
-        <v>0.2162367264830055</v>
+        <v>3.405992878095765e-05</v>
       </c>
       <c r="P14" t="n">
-        <v>0.2214006752348217</v>
+        <v>3.487331385932082e-05</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.1973329171000637</v>
+        <v>3.108234762837578e-05</v>
       </c>
       <c r="R14" t="n">
-        <v>0.1703653896969353</v>
+        <v>2.683463227637121e-05</v>
       </c>
       <c r="S14" t="n">
-        <v>0.180157213043571</v>
+        <v>2.837696419771733e-05</v>
       </c>
       <c r="T14" t="n">
-        <v>0.1995119317244943</v>
+        <v>3.142556907890309e-05</v>
       </c>
       <c r="U14" t="n">
-        <v>0.1736229870271752</v>
+        <v>2.734774369305615e-05</v>
       </c>
       <c r="V14" t="n">
-        <v>0.1432875722655259</v>
+        <v>2.256954489617514e-05</v>
       </c>
       <c r="W14" t="n">
-        <v>0.1207903637408908</v>
+        <v>1.902595943508258e-05</v>
       </c>
       <c r="X14" t="n">
-        <v>0.1061628390457953</v>
+        <v>1.672194541554088e-05</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.1841563558298237</v>
+        <v>2.900687809208695e-05</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.1801445482207373</v>
+        <v>2.837496933324286e-05</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.160405203815859</v>
+        <v>2.526578119694452e-05</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.1494900709662038</v>
+        <v>2.354651429191593e-05</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.171602880760061</v>
+        <v>2.702955225209719e-05</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.2109394804064183</v>
+        <v>3.322554774384948e-05</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.2428108125320964</v>
+        <v>3.824567230830527e-05</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.2466151433424021</v>
+        <v>3.884490093410672e-05</v>
       </c>
       <c r="AG14" t="n">
-        <v>0.233185110075877</v>
+        <v>3.672950645869281e-05</v>
       </c>
       <c r="AH14" t="n">
-        <v>0.3233128324532813</v>
+        <v>5.092572490544945e-05</v>
       </c>
       <c r="AI14" t="n">
-        <v>0.231996455507622</v>
+        <v>3.654227882813068e-05</v>
       </c>
       <c r="AJ14" t="n">
-        <v>0.2054276159988004</v>
+        <v>3.235736169503543e-05</v>
       </c>
       <c r="AK14" t="n">
-        <v>0.220107039725565</v>
+        <v>3.466955044673851e-05</v>
       </c>
       <c r="AL14" t="n">
-        <v>0.2374629565093992</v>
+        <v>3.740331958577551e-05</v>
       </c>
     </row>
     <row r="15">
@@ -2087,115 +2087,115 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.3040969641608656</v>
+        <v>4.789899065845566e-05</v>
       </c>
       <c r="C15" t="n">
-        <v>0.332361031870691</v>
+        <v>5.235092696416217e-05</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3298684273438265</v>
+        <v>5.195831126910923e-05</v>
       </c>
       <c r="E15" t="n">
-        <v>0.3206037601730856</v>
+        <v>5.049901289206174e-05</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2958994156294028</v>
+        <v>4.660777651689303e-05</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2709106056154892</v>
+        <v>4.267173335143351e-05</v>
       </c>
       <c r="H15" t="n">
-        <v>0.2472710339205272</v>
+        <v>3.894821172105018e-05</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1794300953206792</v>
+        <v>2.826243426443602e-05</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1690839481913134</v>
+        <v>2.663278956848192e-05</v>
       </c>
       <c r="K15" t="n">
-        <v>0.1700207012898356</v>
+        <v>2.678033963705695e-05</v>
       </c>
       <c r="L15" t="n">
-        <v>0.1515821945779635</v>
+        <v>2.387604934535699e-05</v>
       </c>
       <c r="M15" t="n">
-        <v>0.09750066847681053</v>
+        <v>1.535754762120358e-05</v>
       </c>
       <c r="N15" t="n">
-        <v>0.1067647465581687</v>
+        <v>1.681675320946931e-05</v>
       </c>
       <c r="O15" t="n">
-        <v>0.1156252933586813</v>
+        <v>1.821239768621604e-05</v>
       </c>
       <c r="P15" t="n">
-        <v>0.1517407799660648</v>
+        <v>2.390102848332436e-05</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.1568085917764956</v>
+        <v>2.469927081776025e-05</v>
       </c>
       <c r="R15" t="n">
-        <v>0.1375781909990072</v>
+        <v>2.167024752664968e-05</v>
       </c>
       <c r="S15" t="n">
-        <v>0.1215405949001535</v>
+        <v>1.914413001724661e-05</v>
       </c>
       <c r="T15" t="n">
-        <v>0.1397762761075372</v>
+        <v>2.201647281163568e-05</v>
       </c>
       <c r="U15" t="n">
-        <v>0.1389967908649278</v>
+        <v>2.189369435359621e-05</v>
       </c>
       <c r="V15" t="n">
-        <v>0.1504143757814247</v>
+        <v>2.369210360364089e-05</v>
       </c>
       <c r="W15" t="n">
-        <v>0.1399813119790815</v>
+        <v>2.204876846878848e-05</v>
       </c>
       <c r="X15" t="n">
-        <v>0.1694628170831471</v>
+        <v>2.669246605213509e-05</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.1586405234729069</v>
+        <v>2.498782246264584e-05</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.179460744430849</v>
+        <v>2.826726187409587e-05</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.1930396627660579</v>
+        <v>3.040610756854364e-05</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.2384481985766279</v>
+        <v>3.755850725989362e-05</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.3025626034827806</v>
+        <v>4.765731008795376e-05</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.3369241061202396</v>
+        <v>5.306966696032124e-05</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.3187691784482184</v>
+        <v>5.021004383528713e-05</v>
       </c>
       <c r="AF15" t="n">
-        <v>0.2617548815919962</v>
+        <v>4.122959485234377e-05</v>
       </c>
       <c r="AG15" t="n">
-        <v>0.1770247711149894</v>
+        <v>2.788356628731953e-05</v>
       </c>
       <c r="AH15" t="n">
-        <v>0.1384479098778964</v>
+        <v>2.180723888587076e-05</v>
       </c>
       <c r="AI15" t="n">
-        <v>0.2195581872704363</v>
+        <v>3.458309947313667e-05</v>
       </c>
       <c r="AJ15" t="n">
-        <v>0.2168851748923208</v>
+        <v>3.416206733530328e-05</v>
       </c>
       <c r="AK15" t="n">
-        <v>0.3618813755533683</v>
+        <v>5.700074209859726e-05</v>
       </c>
       <c r="AL15" t="n">
-        <v>0.3011542161233267</v>
+        <v>4.743547185566452e-05</v>
       </c>
     </row>
     <row r="16">
@@ -2205,115 +2205,115 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.3580281650843918</v>
+        <v>5.639381432880561e-05</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3191676971503628</v>
+        <v>5.027281540436184e-05</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2634822578914997</v>
+        <v>4.150167774360799e-05</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1949638861484612</v>
+        <v>3.070919628260842e-05</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1616246353498621</v>
+        <v>2.545785657598363e-05</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1334818953823281</v>
+        <v>2.102503087340552e-05</v>
       </c>
       <c r="H16" t="n">
-        <v>0.1372841973390792</v>
+        <v>2.162393992996125e-05</v>
       </c>
       <c r="I16" t="n">
-        <v>0.1354584592251756</v>
+        <v>2.133636385006197e-05</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1268157084796323</v>
+        <v>1.997502491540181e-05</v>
       </c>
       <c r="K16" t="n">
-        <v>0.1692071390309354</v>
+        <v>2.665219363222372e-05</v>
       </c>
       <c r="L16" t="n">
-        <v>0.1980646555430562</v>
+        <v>3.119760538157975e-05</v>
       </c>
       <c r="M16" t="n">
-        <v>0.1948024830201132</v>
+        <v>3.068377331609404e-05</v>
       </c>
       <c r="N16" t="n">
-        <v>0.1582516718996468</v>
+        <v>2.492657358458976e-05</v>
       </c>
       <c r="O16" t="n">
-        <v>0.122955722255924</v>
+        <v>1.936702988137917e-05</v>
       </c>
       <c r="P16" t="n">
-        <v>0.1515268585539591</v>
+        <v>2.386733324487182e-05</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.1814319919746178</v>
+        <v>2.857775746863439e-05</v>
       </c>
       <c r="R16" t="n">
-        <v>0.1890933688380198</v>
+        <v>2.978451801563174e-05</v>
       </c>
       <c r="S16" t="n">
-        <v>0.1722085987285993</v>
+        <v>2.71249602394697e-05</v>
       </c>
       <c r="T16" t="n">
-        <v>0.1178099931078734</v>
+        <v>1.855651461341669e-05</v>
       </c>
       <c r="U16" t="n">
-        <v>0.114542668675176</v>
+        <v>1.804187105914192e-05</v>
       </c>
       <c r="V16" t="n">
-        <v>0.09997950978548995</v>
+        <v>1.57479954410819e-05</v>
       </c>
       <c r="W16" t="n">
-        <v>0.08006716274269154</v>
+        <v>1.261155727366113e-05</v>
       </c>
       <c r="X16" t="n">
-        <v>0.09514429448735255</v>
+        <v>1.498638990175601e-05</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.1069005351060816</v>
+        <v>1.683814156632435e-05</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.2567998870196286</v>
+        <v>4.044912261254535e-05</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.246853042285567</v>
+        <v>3.888237292692241e-05</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.377107585950566</v>
+        <v>5.939905643755017e-05</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.4513529193487099</v>
+        <v>7.109360439426824e-05</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.525839127438699</v>
+        <v>8.28260930606096e-05</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.4956867003103818</v>
+        <v>7.807671705373498e-05</v>
       </c>
       <c r="AF16" t="n">
-        <v>0.4272550768520522</v>
+        <v>6.729789950842223e-05</v>
       </c>
       <c r="AG16" t="n">
-        <v>0.3274663207535897</v>
+        <v>5.157995010577482e-05</v>
       </c>
       <c r="AH16" t="n">
-        <v>0.3577915491481246</v>
+        <v>5.635654442526618e-05</v>
       </c>
       <c r="AI16" t="n">
-        <v>0.3044618817058202</v>
+        <v>4.795646963436429e-05</v>
       </c>
       <c r="AJ16" t="n">
-        <v>0.2594290577651311</v>
+        <v>4.086324915710266e-05</v>
       </c>
       <c r="AK16" t="n">
-        <v>0.1586266970609025</v>
+        <v>2.49856446336719e-05</v>
       </c>
       <c r="AL16" t="n">
-        <v>0.2143689070094262</v>
+        <v>3.376572437229631e-05</v>
       </c>
     </row>
     <row r="17">
@@ -2323,115 +2323,115 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.1978361800256182</v>
+        <v>3.116161769355517e-05</v>
       </c>
       <c r="C17" t="n">
-        <v>0.289644798437118</v>
+        <v>4.562259782136688e-05</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3072829225310454</v>
+        <v>4.840081806285798e-05</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2918103245015398</v>
+        <v>4.596369465874113e-05</v>
       </c>
       <c r="F17" t="n">
-        <v>0.2488791950373226</v>
+        <v>3.920151676315487e-05</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1789084909004454</v>
+        <v>2.818027518954644e-05</v>
       </c>
       <c r="H17" t="n">
-        <v>0.1220635531787897</v>
+        <v>1.922650234139093e-05</v>
       </c>
       <c r="I17" t="n">
-        <v>0.133724001444989</v>
+        <v>2.106316553899072e-05</v>
       </c>
       <c r="J17" t="n">
-        <v>0.1571105537387805</v>
+        <v>2.474683351951428e-05</v>
       </c>
       <c r="K17" t="n">
-        <v>0.1539639592504454</v>
+        <v>2.425120640788359e-05</v>
       </c>
       <c r="L17" t="n">
-        <v>0.1383075032131152</v>
+        <v>2.178512311913398e-05</v>
       </c>
       <c r="M17" t="n">
-        <v>0.2057872830586024</v>
+        <v>3.241401365532432e-05</v>
       </c>
       <c r="N17" t="n">
-        <v>0.2617018398721339</v>
+        <v>4.122124013281803e-05</v>
       </c>
       <c r="O17" t="n">
-        <v>0.3369559937861381</v>
+        <v>5.307468965765466e-05</v>
       </c>
       <c r="P17" t="n">
-        <v>0.3888736694036695</v>
+        <v>6.125235846890055e-05</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.407887909361649</v>
+        <v>6.424733378750685e-05</v>
       </c>
       <c r="R17" t="n">
-        <v>0.3634545417420465</v>
+        <v>5.724853501157036e-05</v>
       </c>
       <c r="S17" t="n">
-        <v>0.2775117174348658</v>
+        <v>4.371148918801094e-05</v>
       </c>
       <c r="T17" t="n">
-        <v>0.2697576789362195</v>
+        <v>4.249013330030307e-05</v>
       </c>
       <c r="U17" t="n">
-        <v>0.2320909807305996</v>
+        <v>3.694539939657966e-05</v>
       </c>
       <c r="V17" t="n">
-        <v>0.1856449580103499</v>
+        <v>2.924135113964247e-05</v>
       </c>
       <c r="W17" t="n">
-        <v>0.1748601693666832</v>
+        <v>2.754261504103695e-05</v>
       </c>
       <c r="X17" t="n">
-        <v>0.1688504755015239</v>
+        <v>2.659601476470151e-05</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.1379305153819633</v>
+        <v>2.17257429255417e-05</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.2377244348920983</v>
+        <v>3.744450562867091e-05</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.285298798778524</v>
+        <v>4.493804972788928e-05</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.2853807330664935</v>
+        <v>4.495095538021924e-05</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.2712832584190164</v>
+        <v>4.27304307251618e-05</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.3160296312454475</v>
+        <v>4.977853164891586e-05</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.3092023187470236</v>
+        <v>4.870314643917936e-05</v>
       </c>
       <c r="AF17" t="n">
-        <v>0.2740476920118364</v>
+        <v>4.316586282230159e-05</v>
       </c>
       <c r="AG17" t="n">
-        <v>0.2305899216717844</v>
+        <v>3.632073254847776e-05</v>
       </c>
       <c r="AH17" t="n">
-        <v>0.1535554719746453</v>
+        <v>2.418686466655239e-05</v>
       </c>
       <c r="AI17" t="n">
-        <v>0.1860221394725691</v>
+        <v>2.930076183249576e-05</v>
       </c>
       <c r="AJ17" t="n">
-        <v>0.1799688038358046</v>
+        <v>2.834728744343709e-05</v>
       </c>
       <c r="AK17" t="n">
-        <v>0.1611645293139988</v>
+        <v>2.538538424869641e-05</v>
       </c>
       <c r="AL17" t="n">
-        <v>0.1258536703791298</v>
+        <v>1.982349214980449e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>